<commit_message>
Finish create new propety and verity
</commit_message>
<xml_diff>
--- a/Keys_Onboarding/ExcelData/TestData.xlsx
+++ b/Keys_Onboarding/ExcelData/TestData.xlsx
@@ -1,16 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D355EFF-1A9B-44A7-98A4-0316830708D9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20736" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
     <sheet name="Register" sheetId="2" r:id="rId2"/>
     <sheet name="PropertyDetails" sheetId="4" r:id="rId3"/>
     <sheet name="FinanceDetails" sheetId="5" r:id="rId4"/>
+    <sheet name="TenantDetails" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
   <si>
     <t>Url</t>
   </si>
@@ -126,9 +128,6 @@
     <t>YearBuilt</t>
   </si>
   <si>
-    <t>D:\Users\Morgan\Source\Repos\ICOnboardingTask\Keys_Onboarding\Photos\01.jpeg</t>
-  </si>
-  <si>
     <t>Bedrooms</t>
   </si>
   <si>
@@ -151,17 +150,69 @@
   </si>
   <si>
     <t>Duration</t>
+  </si>
+  <si>
+    <t>C:\Users\Mogan\source\repos\ICOnboardingTask\Keys_Onboarding\Photos\01.jpeg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LastName</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Paymentfrequency</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PaymentDueDay</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TenantEmail</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IsMainTenant</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>test@test.com</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>test</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fortnightly</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FirstName</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Duraion</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RentAmount</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -174,7 +225,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -204,7 +255,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -213,10 +264,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -493,21 +547,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.42578125" customWidth="1"/>
-    <col min="2" max="2" width="36.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="1" max="1" width="47.44140625" customWidth="1"/>
+    <col min="2" max="2" width="36.44140625" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -518,7 +572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -529,7 +583,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -543,10 +597,10 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="B3" r:id="rId3"/>
-    <hyperlink ref="A3" r:id="rId4"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
@@ -554,23 +608,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -587,7 +641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -607,40 +661,38 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="79" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="2"/>
+    <col min="14" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -660,7 +712,7 @@
         <v>18</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>27</v>
@@ -681,7 +733,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -719,7 +771,7 @@
         <v>26</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -729,43 +781,43 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="13.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="E1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>500</v>
       </c>
@@ -776,7 +828,7 @@
         <v>450</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E2" s="3">
         <v>300</v>
@@ -786,6 +838,90 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61724BB8-997A-436C-BF1D-5E5F046F5812}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="8.88671875" style="2"/>
+    <col min="3" max="3" width="10.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="2">
+        <v>125</v>
+      </c>
+      <c r="F2" s="2">
+        <v>23</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="2">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{B5785CEA-4456-42FD-9820-F38C1B1323A1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>